<commit_message>
update buku tesis dan tambah data
</commit_message>
<xml_diff>
--- a/data/berita 2020.xlsx
+++ b/data/berita 2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\bimbingan\catatanbimbingan\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ACFF09-EE87-4BC8-82BF-BC9F58C61D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0873BD9-F426-4D27-A5CA-CA92B2435C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{2006F5EE-FD3A-4956-8B23-E6D8A3D57128}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'2020antaranews'!$A$1:$D$159</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2020pikiranrakyat'!$A$1:$D$237</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020tribunnews'!$A$1:$D$165</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'2020tribunnews'!$A$1:$D$164</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="575">
   <si>
     <t>positive</t>
   </si>
@@ -1794,12 +1794,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1815,10 +1821,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2263,8 +2270,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D237"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="C215" sqref="C215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3196,7 +3203,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>8</v>
       </c>
@@ -4022,17 +4029,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126">
-        <v>1</v>
-      </c>
-      <c r="B126">
-        <v>17</v>
-      </c>
-      <c r="C126" t="s">
+    <row r="126" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3">
+        <v>1</v>
+      </c>
+      <c r="B126" s="3">
+        <v>17</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4960,7 +4967,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>7</v>
       </c>
@@ -5613,10 +5620,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B534B9-0422-4910-9F73-01CC608C08CC}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D164"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C168" sqref="C168"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5865,13 +5872,13 @@
     </row>
     <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -5879,13 +5886,13 @@
     </row>
     <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -5893,13 +5900,13 @@
     </row>
     <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -5907,13 +5914,13 @@
     </row>
     <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -5921,13 +5928,13 @@
     </row>
     <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -5935,13 +5942,13 @@
     </row>
     <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -5949,13 +5956,13 @@
     </row>
     <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B24">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
@@ -5963,13 +5970,13 @@
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B25">
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -5980,10 +5987,10 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -5991,13 +5998,13 @@
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -6008,10 +6015,10 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -6019,86 +6026,86 @@
     </row>
     <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B29">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B30">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B32">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33">
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B34">
         <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -6109,7 +6116,7 @@
         <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -6117,13 +6124,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36">
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -6131,13 +6138,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B37">
         <v>17</v>
       </c>
       <c r="C37" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
@@ -6145,13 +6152,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B38">
         <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D38" t="s">
         <v>7</v>
@@ -6159,13 +6166,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39">
         <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -6173,13 +6180,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B40">
         <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -6187,30 +6194,30 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B41">
         <v>17</v>
       </c>
       <c r="C41" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B42">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6218,10 +6225,10 @@
         <v>12</v>
       </c>
       <c r="B43">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C43" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
@@ -6229,13 +6236,13 @@
     </row>
     <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44">
-        <v>17</v>
-      </c>
-      <c r="C44" t="s">
-        <v>289</v>
+        <v>3</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="D44" t="s">
         <v>10</v>
@@ -6243,16 +6250,16 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>290</v>
+        <v>17</v>
+      </c>
+      <c r="C45" t="s">
+        <v>291</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -6263,7 +6270,7 @@
         <v>17</v>
       </c>
       <c r="C46" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -6271,13 +6278,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B47">
         <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -6285,13 +6292,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B48">
         <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -6305,7 +6312,7 @@
         <v>17</v>
       </c>
       <c r="C49" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
@@ -6313,13 +6320,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B50">
         <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
@@ -6333,7 +6340,7 @@
         <v>17</v>
       </c>
       <c r="C51" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -6347,7 +6354,7 @@
         <v>17</v>
       </c>
       <c r="C52" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
@@ -6355,13 +6362,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B53">
         <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D53" t="s">
         <v>7</v>
@@ -6375,7 +6382,7 @@
         <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -6389,7 +6396,7 @@
         <v>17</v>
       </c>
       <c r="C55" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
@@ -6397,13 +6404,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56">
         <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
@@ -6417,7 +6424,7 @@
         <v>17</v>
       </c>
       <c r="C57" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -6425,13 +6432,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B58">
         <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D58" t="s">
         <v>7</v>
@@ -6439,13 +6446,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B59">
         <v>17</v>
       </c>
       <c r="C59" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -6453,13 +6460,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B60">
         <v>17</v>
       </c>
       <c r="C60" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -6467,13 +6474,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B61">
         <v>17</v>
       </c>
       <c r="C61" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D61" t="s">
         <v>7</v>
@@ -6481,13 +6488,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B62">
         <v>17</v>
       </c>
       <c r="C62" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -6495,13 +6502,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B63">
         <v>17</v>
       </c>
       <c r="C63" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
@@ -6515,7 +6522,7 @@
         <v>17</v>
       </c>
       <c r="C64" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D64" t="s">
         <v>7</v>
@@ -6529,7 +6536,7 @@
         <v>17</v>
       </c>
       <c r="C65" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
@@ -6537,13 +6544,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B66">
         <v>17</v>
       </c>
       <c r="C66" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -6551,13 +6558,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B67">
         <v>17</v>
       </c>
       <c r="C67" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D67" t="s">
         <v>7</v>
@@ -6571,7 +6578,7 @@
         <v>17</v>
       </c>
       <c r="C68" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D68" t="s">
         <v>7</v>
@@ -6585,7 +6592,7 @@
         <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -6599,7 +6606,7 @@
         <v>17</v>
       </c>
       <c r="C70" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D70" t="s">
         <v>7</v>
@@ -6607,13 +6614,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B71">
         <v>17</v>
       </c>
       <c r="C71" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D71" t="s">
         <v>7</v>
@@ -6621,13 +6628,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B72">
         <v>17</v>
       </c>
       <c r="C72" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -6635,13 +6642,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B73">
         <v>17</v>
       </c>
       <c r="C73" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -6655,7 +6662,7 @@
         <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="D74" t="s">
         <v>7</v>
@@ -6663,13 +6670,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75">
         <v>17</v>
       </c>
       <c r="C75" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
@@ -6683,7 +6690,7 @@
         <v>17</v>
       </c>
       <c r="C76" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
@@ -6691,13 +6698,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B77">
         <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D77" t="s">
         <v>7</v>
@@ -6705,13 +6712,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B78">
         <v>17</v>
       </c>
       <c r="C78" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -6719,13 +6726,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B79">
         <v>17</v>
       </c>
       <c r="C79" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -6733,13 +6740,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B80">
         <v>17</v>
       </c>
       <c r="C80" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D80" t="s">
         <v>7</v>
@@ -6747,13 +6754,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B81">
         <v>17</v>
       </c>
       <c r="C81" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -6761,13 +6768,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B82">
         <v>17</v>
       </c>
       <c r="C82" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -6781,7 +6788,7 @@
         <v>17</v>
       </c>
       <c r="C83" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D83" t="s">
         <v>7</v>
@@ -6789,13 +6796,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B84">
         <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D84" t="s">
         <v>7</v>
@@ -6809,35 +6816,35 @@
         <v>17</v>
       </c>
       <c r="C85" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D85" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B86">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C86" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D86" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B87">
         <v>28</v>
       </c>
-      <c r="C87" t="s">
-        <v>330</v>
+      <c r="C87" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="D87" t="s">
         <v>10</v>
@@ -6845,13 +6852,13 @@
     </row>
     <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B88">
         <v>28</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>331</v>
+      <c r="C88" t="s">
+        <v>332</v>
       </c>
       <c r="D88" t="s">
         <v>10</v>
@@ -6859,13 +6866,13 @@
     </row>
     <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B89">
         <v>28</v>
       </c>
       <c r="C89" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D89" t="s">
         <v>10</v>
@@ -6873,13 +6880,13 @@
     </row>
     <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B90">
         <v>28</v>
       </c>
       <c r="C90" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D90" t="s">
         <v>10</v>
@@ -6887,13 +6894,13 @@
     </row>
     <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B91">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D91" t="s">
         <v>10</v>
@@ -6901,13 +6908,13 @@
     </row>
     <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B92">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D92" t="s">
         <v>10</v>
@@ -6918,10 +6925,10 @@
         <v>11</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C93" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D93" t="s">
         <v>10</v>
@@ -6935,7 +6942,7 @@
         <v>16</v>
       </c>
       <c r="C94" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D94" t="s">
         <v>10</v>
@@ -6949,38 +6956,38 @@
         <v>16</v>
       </c>
       <c r="C95" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D95" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>11</v>
       </c>
       <c r="B96">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C96" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B97">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C97" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D97" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6991,7 +6998,7 @@
         <v>16</v>
       </c>
       <c r="C98" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D98" t="s">
         <v>10</v>
@@ -7005,7 +7012,7 @@
         <v>16</v>
       </c>
       <c r="C99" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D99" t="s">
         <v>10</v>
@@ -7019,38 +7026,38 @@
         <v>16</v>
       </c>
       <c r="C100" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D100" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>10</v>
       </c>
       <c r="B101">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C101" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D101" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>10</v>
       </c>
       <c r="B102">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C102" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D102" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -7061,7 +7068,7 @@
         <v>16</v>
       </c>
       <c r="C103" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D103" t="s">
         <v>10</v>
@@ -7075,7 +7082,7 @@
         <v>16</v>
       </c>
       <c r="C104" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D104" t="s">
         <v>10</v>
@@ -7089,7 +7096,7 @@
         <v>16</v>
       </c>
       <c r="C105" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D105" t="s">
         <v>10</v>
@@ -7103,7 +7110,7 @@
         <v>16</v>
       </c>
       <c r="C106" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="D106" t="s">
         <v>10</v>
@@ -7114,10 +7121,10 @@
         <v>10</v>
       </c>
       <c r="B107">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D107" t="s">
         <v>10</v>
@@ -7128,10 +7135,10 @@
         <v>10</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C108" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D108" t="s">
         <v>10</v>
@@ -7145,7 +7152,7 @@
         <v>16</v>
       </c>
       <c r="C109" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D109" t="s">
         <v>10</v>
@@ -7159,7 +7166,7 @@
         <v>16</v>
       </c>
       <c r="C110" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D110" t="s">
         <v>10</v>
@@ -7173,7 +7180,7 @@
         <v>16</v>
       </c>
       <c r="C111" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D111" t="s">
         <v>10</v>
@@ -7187,7 +7194,7 @@
         <v>16</v>
       </c>
       <c r="C112" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="D112" t="s">
         <v>10</v>
@@ -7200,8 +7207,8 @@
       <c r="B113">
         <v>16</v>
       </c>
-      <c r="C113" t="s">
-        <v>356</v>
+      <c r="C113" s="2" t="s">
+        <v>357</v>
       </c>
       <c r="D113" t="s">
         <v>10</v>
@@ -7214,8 +7221,8 @@
       <c r="B114">
         <v>16</v>
       </c>
-      <c r="C114" s="2" t="s">
-        <v>357</v>
+      <c r="C114" t="s">
+        <v>358</v>
       </c>
       <c r="D114" t="s">
         <v>10</v>
@@ -7229,7 +7236,7 @@
         <v>16</v>
       </c>
       <c r="C115" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D115" t="s">
         <v>10</v>
@@ -7243,7 +7250,7 @@
         <v>16</v>
       </c>
       <c r="C116" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D116" t="s">
         <v>10</v>
@@ -7257,7 +7264,7 @@
         <v>16</v>
       </c>
       <c r="C117" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D117" t="s">
         <v>10</v>
@@ -7271,7 +7278,7 @@
         <v>16</v>
       </c>
       <c r="C118" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D118" t="s">
         <v>10</v>
@@ -7285,7 +7292,7 @@
         <v>16</v>
       </c>
       <c r="C119" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D119" t="s">
         <v>10</v>
@@ -7299,7 +7306,7 @@
         <v>16</v>
       </c>
       <c r="C120" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="D120" t="s">
         <v>10</v>
@@ -7313,7 +7320,7 @@
         <v>16</v>
       </c>
       <c r="C121" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D121" t="s">
         <v>10</v>
@@ -7327,7 +7334,7 @@
         <v>16</v>
       </c>
       <c r="C122" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D122" t="s">
         <v>10</v>
@@ -7341,7 +7348,7 @@
         <v>16</v>
       </c>
       <c r="C123" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D123" t="s">
         <v>10</v>
@@ -7355,7 +7362,7 @@
         <v>16</v>
       </c>
       <c r="C124" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D124" t="s">
         <v>10</v>
@@ -7369,7 +7376,7 @@
         <v>16</v>
       </c>
       <c r="C125" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D125" t="s">
         <v>10</v>
@@ -7383,7 +7390,7 @@
         <v>16</v>
       </c>
       <c r="C126" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D126" t="s">
         <v>10</v>
@@ -7397,7 +7404,7 @@
         <v>16</v>
       </c>
       <c r="C127" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D127" t="s">
         <v>10</v>
@@ -7411,7 +7418,7 @@
         <v>16</v>
       </c>
       <c r="C128" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D128" t="s">
         <v>10</v>
@@ -7425,7 +7432,7 @@
         <v>16</v>
       </c>
       <c r="C129" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D129" t="s">
         <v>10</v>
@@ -7439,7 +7446,7 @@
         <v>16</v>
       </c>
       <c r="C130" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D130" t="s">
         <v>10</v>
@@ -7453,7 +7460,7 @@
         <v>16</v>
       </c>
       <c r="C131" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D131" t="s">
         <v>10</v>
@@ -7467,7 +7474,7 @@
         <v>16</v>
       </c>
       <c r="C132" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="D132" t="s">
         <v>10</v>
@@ -7481,7 +7488,7 @@
         <v>16</v>
       </c>
       <c r="C133" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D133" t="s">
         <v>10</v>
@@ -7495,7 +7502,7 @@
         <v>16</v>
       </c>
       <c r="C134" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="D134" t="s">
         <v>10</v>
@@ -7509,7 +7516,7 @@
         <v>16</v>
       </c>
       <c r="C135" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D135" t="s">
         <v>10</v>
@@ -7523,7 +7530,7 @@
         <v>16</v>
       </c>
       <c r="C136" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D136" t="s">
         <v>10</v>
@@ -7537,7 +7544,7 @@
         <v>16</v>
       </c>
       <c r="C137" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D137" t="s">
         <v>10</v>
@@ -7551,7 +7558,7 @@
         <v>16</v>
       </c>
       <c r="C138" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="D138" t="s">
         <v>10</v>
@@ -7564,8 +7571,8 @@
       <c r="B139">
         <v>16</v>
       </c>
-      <c r="C139" t="s">
-        <v>382</v>
+      <c r="C139" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="D139" t="s">
         <v>10</v>
@@ -7573,13 +7580,13 @@
     </row>
     <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B140">
         <v>16</v>
       </c>
-      <c r="C140" s="2" t="s">
-        <v>383</v>
+      <c r="C140" t="s">
+        <v>384</v>
       </c>
       <c r="D140" t="s">
         <v>10</v>
@@ -7593,7 +7600,7 @@
         <v>16</v>
       </c>
       <c r="C141" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D141" t="s">
         <v>10</v>
@@ -7607,7 +7614,7 @@
         <v>16</v>
       </c>
       <c r="C142" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D142" t="s">
         <v>10</v>
@@ -7621,7 +7628,7 @@
         <v>16</v>
       </c>
       <c r="C143" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D143" t="s">
         <v>10</v>
@@ -7635,7 +7642,7 @@
         <v>16</v>
       </c>
       <c r="C144" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D144" t="s">
         <v>10</v>
@@ -7643,13 +7650,13 @@
     </row>
     <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B145">
         <v>16</v>
       </c>
       <c r="C145" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D145" t="s">
         <v>10</v>
@@ -7663,7 +7670,7 @@
         <v>16</v>
       </c>
       <c r="C146" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="D146" t="s">
         <v>10</v>
@@ -7677,7 +7684,7 @@
         <v>16</v>
       </c>
       <c r="C147" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D147" t="s">
         <v>10</v>
@@ -7685,13 +7692,13 @@
     </row>
     <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B148">
         <v>16</v>
       </c>
       <c r="C148" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D148" t="s">
         <v>10</v>
@@ -7705,7 +7712,7 @@
         <v>16</v>
       </c>
       <c r="C149" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D149" t="s">
         <v>10</v>
@@ -7719,7 +7726,7 @@
         <v>16</v>
       </c>
       <c r="C150" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D150" t="s">
         <v>10</v>
@@ -7733,7 +7740,7 @@
         <v>16</v>
       </c>
       <c r="C151" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D151" t="s">
         <v>10</v>
@@ -7747,7 +7754,7 @@
         <v>16</v>
       </c>
       <c r="C152" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D152" t="s">
         <v>10</v>
@@ -7761,7 +7768,7 @@
         <v>16</v>
       </c>
       <c r="C153" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D153" t="s">
         <v>10</v>
@@ -7775,7 +7782,7 @@
         <v>16</v>
       </c>
       <c r="C154" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D154" t="s">
         <v>10</v>
@@ -7783,13 +7790,13 @@
     </row>
     <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B155">
         <v>16</v>
       </c>
       <c r="C155" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D155" t="s">
         <v>10</v>
@@ -7803,7 +7810,7 @@
         <v>16</v>
       </c>
       <c r="C156" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D156" t="s">
         <v>10</v>
@@ -7811,13 +7818,13 @@
     </row>
     <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B157">
         <v>16</v>
       </c>
       <c r="C157" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D157" t="s">
         <v>10</v>
@@ -7825,13 +7832,13 @@
     </row>
     <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B158">
         <v>16</v>
       </c>
       <c r="C158" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D158" t="s">
         <v>10</v>
@@ -7839,30 +7846,30 @@
     </row>
     <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B159">
         <v>16</v>
       </c>
       <c r="C159" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D159" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B160">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C160" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D160" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -7873,35 +7880,35 @@
         <v>17</v>
       </c>
       <c r="C161" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D161" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2</v>
       </c>
       <c r="B162">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C162" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D162" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B163">
         <v>16</v>
       </c>
       <c r="C163" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D163" t="s">
         <v>10</v>
@@ -7915,28 +7922,14 @@
         <v>16</v>
       </c>
       <c r="C164" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="D164" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165">
-        <v>9</v>
-      </c>
-      <c r="B165">
-        <v>16</v>
-      </c>
-      <c r="C165" t="s">
-        <v>408</v>
-      </c>
-      <c r="D165" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D165" xr:uid="{61B534B9-0422-4910-9F73-01CC608C08CC}">
+  <autoFilter ref="A1:D164" xr:uid="{61B534B9-0422-4910-9F73-01CC608C08CC}">
     <filterColumn colId="3">
       <filters>
         <filter val="positif"/>
@@ -7944,10 +7937,10 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="C88" r:id="rId1" xr:uid="{878AC756-607F-45CC-9F8A-CB6AC04782BB}"/>
-    <hyperlink ref="C114" r:id="rId2" xr:uid="{7DEBB254-CA11-4894-82D0-48A288DC1B6D}"/>
-    <hyperlink ref="C140" r:id="rId3" xr:uid="{69CC1DE4-828F-42E3-A54B-7E769551CA57}"/>
-    <hyperlink ref="C45" r:id="rId4" xr:uid="{FE5C9E5D-A323-488D-8125-3F71EF4A8478}"/>
+    <hyperlink ref="C87" r:id="rId1" xr:uid="{878AC756-607F-45CC-9F8A-CB6AC04782BB}"/>
+    <hyperlink ref="C113" r:id="rId2" xr:uid="{7DEBB254-CA11-4894-82D0-48A288DC1B6D}"/>
+    <hyperlink ref="C139" r:id="rId3" xr:uid="{69CC1DE4-828F-42E3-A54B-7E769551CA57}"/>
+    <hyperlink ref="C44" r:id="rId4" xr:uid="{FE5C9E5D-A323-488D-8125-3F71EF4A8478}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7958,8 +7951,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7981,7 +7974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -7995,7 +7988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -8009,7 +8002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -8023,7 +8016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -8037,7 +8030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -8051,7 +8044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12</v>
       </c>
@@ -8065,7 +8058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -8079,7 +8072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -8093,7 +8086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -8107,7 +8100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -8121,7 +8114,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -8135,7 +8128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -8149,7 +8142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -8163,7 +8156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -8177,7 +8170,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -8191,7 +8184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -8205,7 +8198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -8219,7 +8212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -8233,7 +8226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -8247,7 +8240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11</v>
       </c>
@@ -8261,7 +8254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -8275,7 +8268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
@@ -8289,7 +8282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
@@ -8303,7 +8296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -8317,7 +8310,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10</v>
       </c>
@@ -8331,7 +8324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -8345,7 +8338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -8359,7 +8352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -8373,7 +8366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -8387,7 +8380,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -8401,7 +8394,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -8415,7 +8408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -8429,7 +8422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -8443,7 +8436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -8457,7 +8450,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -8471,7 +8464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -8485,7 +8478,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -8499,7 +8492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9</v>
       </c>
@@ -8513,7 +8506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7</v>
       </c>
@@ -8527,7 +8520,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -8541,7 +8534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -8555,7 +8548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>11</v>
       </c>
@@ -8569,7 +8562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9</v>
       </c>
@@ -8583,7 +8576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>8</v>
       </c>
@@ -8597,7 +8590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5</v>
       </c>
@@ -8611,7 +8604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -8625,7 +8618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -8639,7 +8632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9</v>
       </c>
@@ -8653,7 +8646,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>8</v>
       </c>
@@ -8667,7 +8660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -8681,7 +8674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>11</v>
       </c>
@@ -8695,7 +8688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>11</v>
       </c>
@@ -8709,7 +8702,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>11</v>
       </c>
@@ -8723,7 +8716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>10</v>
       </c>
@@ -8737,7 +8730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>10</v>
       </c>
@@ -8751,7 +8744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>10</v>
       </c>
@@ -8765,7 +8758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9</v>
       </c>
@@ -8779,7 +8772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8</v>
       </c>
@@ -8793,7 +8786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7</v>
       </c>
@@ -8807,7 +8800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6</v>
       </c>
@@ -8821,7 +8814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6</v>
       </c>
@@ -8835,7 +8828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>3</v>
       </c>
@@ -8849,7 +8842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1</v>
       </c>
@@ -8863,7 +8856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>12</v>
       </c>
@@ -8877,7 +8870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>8</v>
       </c>
@@ -8891,7 +8884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7</v>
       </c>
@@ -8905,7 +8898,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>7</v>
       </c>
@@ -8919,7 +8912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>7</v>
       </c>
@@ -8933,7 +8926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>7</v>
       </c>
@@ -8947,7 +8940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>7</v>
       </c>
@@ -8961,7 +8954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>6</v>
       </c>
@@ -8975,7 +8968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>6</v>
       </c>
@@ -8989,7 +8982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>6</v>
       </c>
@@ -9003,7 +8996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5</v>
       </c>
@@ -9017,7 +9010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5</v>
       </c>
@@ -9031,7 +9024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5</v>
       </c>
@@ -9045,7 +9038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5</v>
       </c>
@@ -9059,7 +9052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5</v>
       </c>
@@ -9073,7 +9066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>5</v>
       </c>
@@ -9087,7 +9080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>5</v>
       </c>
@@ -9101,7 +9094,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>5</v>
       </c>
@@ -9115,7 +9108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5</v>
       </c>
@@ -9129,7 +9122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>5</v>
       </c>
@@ -9143,7 +9136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>5</v>
       </c>
@@ -9157,7 +9150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5</v>
       </c>
@@ -9171,7 +9164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>4</v>
       </c>
@@ -9185,7 +9178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>4</v>
       </c>
@@ -9199,7 +9192,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>4</v>
       </c>
@@ -9213,7 +9206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>4</v>
       </c>
@@ -9227,7 +9220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>4</v>
       </c>
@@ -9241,7 +9234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>4</v>
       </c>
@@ -9255,7 +9248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>4</v>
       </c>
@@ -9269,7 +9262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>3</v>
       </c>
@@ -9283,7 +9276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>3</v>
       </c>
@@ -9297,7 +9290,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>3</v>
       </c>
@@ -9311,7 +9304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>3</v>
       </c>
@@ -9325,7 +9318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>3</v>
       </c>
@@ -9339,7 +9332,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2</v>
       </c>
@@ -9353,7 +9346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2</v>
       </c>
@@ -9367,7 +9360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2</v>
       </c>
@@ -9381,7 +9374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2</v>
       </c>
@@ -9395,7 +9388,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2</v>
       </c>
@@ -9409,7 +9402,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2</v>
       </c>
@@ -9423,7 +9416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2</v>
       </c>
@@ -9437,7 +9430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1</v>
       </c>
@@ -9451,7 +9444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1</v>
       </c>
@@ -9465,7 +9458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1</v>
       </c>
@@ -9479,7 +9472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1</v>
       </c>
@@ -9493,7 +9486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1</v>
       </c>
@@ -9507,7 +9500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1</v>
       </c>
@@ -9521,7 +9514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1</v>
       </c>
@@ -9535,7 +9528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1</v>
       </c>
@@ -9549,7 +9542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>8</v>
       </c>
@@ -9563,7 +9556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>3</v>
       </c>
@@ -9577,7 +9570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>3</v>
       </c>
@@ -9591,7 +9584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>3</v>
       </c>
@@ -9605,7 +9598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>3</v>
       </c>
@@ -9619,7 +9612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>12</v>
       </c>
@@ -9633,7 +9626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>12</v>
       </c>
@@ -9647,7 +9640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>12</v>
       </c>
@@ -9661,7 +9654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>12</v>
       </c>
@@ -9675,7 +9668,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>12</v>
       </c>
@@ -9689,7 +9682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>12</v>
       </c>
@@ -9703,7 +9696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>12</v>
       </c>
@@ -9717,7 +9710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>12</v>
       </c>
@@ -9731,7 +9724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>12</v>
       </c>
@@ -9745,7 +9738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>12</v>
       </c>
@@ -9759,7 +9752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>12</v>
       </c>
@@ -9773,7 +9766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>12</v>
       </c>
@@ -9787,7 +9780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>12</v>
       </c>
@@ -9801,7 +9794,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>12</v>
       </c>
@@ -9815,7 +9808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>12</v>
       </c>
@@ -9829,7 +9822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>12</v>
       </c>
@@ -9843,7 +9836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>12</v>
       </c>
@@ -9857,7 +9850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>12</v>
       </c>
@@ -9871,7 +9864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>11</v>
       </c>
@@ -9885,7 +9878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>11</v>
       </c>
@@ -9899,7 +9892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>11</v>
       </c>
@@ -9913,7 +9906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>11</v>
       </c>
@@ -9927,7 +9920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>10</v>
       </c>
@@ -9941,7 +9934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>10</v>
       </c>
@@ -9955,7 +9948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>10</v>
       </c>
@@ -9969,7 +9962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>10</v>
       </c>
@@ -9983,7 +9976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>10</v>
       </c>
@@ -9997,7 +9990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>10</v>
       </c>
@@ -10011,7 +10004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>10</v>
       </c>
@@ -10025,7 +10018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>10</v>
       </c>
@@ -10039,7 +10032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>10</v>
       </c>
@@ -10053,7 +10046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>10</v>
       </c>
@@ -10067,7 +10060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>9</v>
       </c>
@@ -10081,7 +10074,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>9</v>
       </c>
@@ -10095,7 +10088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>7</v>
       </c>
@@ -10109,7 +10102,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>7</v>
       </c>
@@ -10123,7 +10116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>6</v>
       </c>
@@ -10137,7 +10130,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>6</v>
       </c>
@@ -10151,7 +10144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>6</v>
       </c>
@@ -10165,7 +10158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>5</v>
       </c>
@@ -10179,7 +10172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>9</v>
       </c>
@@ -10197,7 +10190,7 @@
   <autoFilter ref="A1:D159" xr:uid="{4F07AA29-2AF7-45EB-B07F-064A18A20F9D}">
     <filterColumn colId="3">
       <filters>
-        <filter val="positif"/>
+        <filter val="negatif"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D159">
@@ -10208,6 +10201,7 @@
     <hyperlink ref="C30" r:id="rId1" xr:uid="{137F88FA-0BAC-46EF-AE81-A45EE568C155}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10216,7 +10210,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>